<commit_message>
After clone. commit excel
</commit_message>
<xml_diff>
--- a/CodeChamps_Dsalgo/src/test/resources/Exceldata/LoginData.xlsx
+++ b/CodeChamps_Dsalgo/src/test/resources/Exceldata/LoginData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajas\eclipse-workspace\DSalgo_CrossBrowser\CodeChamps_Dsalgo\src\test\resources\Exceldata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mahi\Code\codechamps\CodeChamps_Dsalgo\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BFC00D-0B16-4146-AA8A-EF3DF9920EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B25A6-1235-4A29-8D9C-177B730414C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="4080" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32235" yWindow="2415" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -394,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -466,4 +467,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B929DFD-7344-4087-BE24-79F8D3C70D5D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>